<commit_message>
Added owner to Certificates and Course Track Tests
</commit_message>
<xml_diff>
--- a/TelerikAcademyLearningSystem.Tests/TelerikAcademyLearningSystem.Tests/bin/Debug/report.xlsx
+++ b/TelerikAcademyLearningSystem.Tests/TelerikAcademyLearningSystem.Tests/bin/Debug/report.xlsx
@@ -14,36 +14,51 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
-  <si>
-    <t>Трите имена</t>
-  </si>
-  <si>
-    <t>Потребител</t>
-  </si>
-  <si>
-    <t>Специалност</t>
-  </si>
-  <si>
-    <t>Дата на подаване</t>
-  </si>
-  <si>
-    <t>Статус</t>
-  </si>
-  <si>
-    <t>Ffdsfds Gfgdgfd Gfggsdfgsdf</t>
-  </si>
-  <si>
-    <t>hiksatest</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+  <si>
+    <t>№</t>
+  </si>
+  <si>
+    <t>Име (BG)</t>
+  </si>
+  <si>
+    <t>Име (EN)</t>
+  </si>
+  <si>
+    <t>URL име</t>
+  </si>
+  <si>
+    <t>Описание</t>
+  </si>
+  <si>
+    <t>Валиден за сезон</t>
+  </si>
+  <si>
+    <t>Сертификати</t>
+  </si>
+  <si>
+    <t>Активен?</t>
+  </si>
+  <si>
+    <t>Име на сертификат</t>
   </si>
   <si>
     <t>QA Инженер</t>
   </si>
   <si>
-    <t>ьяа ьяа</t>
-  </si>
-  <si>
-    <t>testStudent</t>
+    <t>QA Engineer</t>
+  </si>
+  <si>
+    <t>asd</t>
+  </si>
+  <si>
+    <t>asdasdasdasd</t>
+  </si>
+  <si>
+    <t>Всички сезони</t>
+  </si>
+  <si>
+    <t/>
   </si>
 </sst>
 </file>
@@ -92,10 +107,9 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf xfId="0" fontId="1" applyFont="1" fillId="2" applyFill="1"/>
-    <xf xfId="0" numFmtId="14" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -115,11 +129,15 @@
   </sheetViews>
   <sheetFormatPr x14ac:dyDescent="0.25" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" customWidth="1" width="27.714285714285715" bestFit="1"/>
-    <col min="2" max="2" customWidth="1" width="11.714285714285714" bestFit="1"/>
+    <col min="1" max="1" customWidth="1" width="1.7142857142857142" bestFit="1"/>
+    <col min="2" max="2" customWidth="1" width="10.714285714285714" bestFit="1"/>
     <col min="3" max="3" customWidth="1" width="11.714285714285714" bestFit="1"/>
-    <col min="4" max="4" customWidth="1" width="53.714285714285715" bestFit="1"/>
-    <col min="5" max="5" customWidth="1" width="6.714285714285714" bestFit="1"/>
+    <col min="4" max="4" customWidth="1" width="7.714285714285714" bestFit="1"/>
+    <col min="5" max="5" customWidth="1" width="12.714285714285714" bestFit="1"/>
+    <col min="6" max="6" customWidth="1" width="16.714285714285715" bestFit="1"/>
+    <col min="7" max="7" customWidth="1" width="11.714285714285714" bestFit="1"/>
+    <col min="8" max="8" customWidth="1" width="8.714285714285714" bestFit="1"/>
+    <col min="9" max="9" customWidth="1" width="17.714285714285715" bestFit="1"/>
   </cols>
   <sheetData>
     <row r="1" x14ac:dyDescent="0.25">
@@ -138,37 +156,46 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>5</v>
+      <c r="A2" t="n">
+        <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="2">
-        <v>42355.75059059028</v>
-      </c>
-      <c r="E2"/>
-    </row>
-    <row r="3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="2">
-        <v>42339.847349537034</v>
-      </c>
-      <c r="E3" t="b">
+        <v>10</v>
+      </c>
+      <c r="D2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" t="n">
         <v>1</v>
+      </c>
+      <c r="H2" t="b">
+        <v>1</v>
+      </c>
+      <c r="I2" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>